<commit_message>
b4 and b6 fixed
</commit_message>
<xml_diff>
--- a/blacktoor/evidence.xlsx
+++ b/blacktoor/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caner\Desktop\testnets\game-of-nfts\blacktoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C41A1CB-A129-412B-8B7C-3EADEDE2ACA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A77EBB2-9623-4DEC-A151-6B9DEACD2BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>3E0F520CAD0D3B2FCAA8EE4A7F869D258418A66544594B1102251F290C4BC5F9</t>
   </si>
   <si>
-    <t>42164D915140A79A2F8B72AF0CC1A8FD1506555282D2438450BBC13E6199D947</t>
-  </si>
-  <si>
     <t>gon-flixnet-1</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>ED7844969AC4C38EC43ECE96DDDD8C98F3CD083DC062E90DE9CC98375A8BA6AC</t>
+  </si>
+  <si>
+    <t>ibc/42164D915140A79A2F8B72AF0CC1A8FD1506555282D2438450BBC13E6199D947</t>
   </si>
 </sst>
 </file>
@@ -824,10 +824,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -862,10 +862,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -900,10 +900,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -938,10 +938,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -976,15 +976,77 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
@@ -992,15 +1054,15 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>46</v>
@@ -1011,8 +1073,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1038,43 +1100,43 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1100,15 +1162,15 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -1116,15 +1178,15 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -1135,8 +1197,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1162,23 +1224,85 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1186,26 +1310,63 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,15 +1385,93 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
@@ -1240,192 +1479,31 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>46</v>
@@ -1436,84 +1514,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
@@ -1537,12 +1537,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1573,12 +1573,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1609,12 +1609,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1645,12 +1645,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1662,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1E91-8CF7-4C20-92C6-08B3D6A5F589}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1675,12 +1675,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1802,7 +1802,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,13 +1831,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
@@ -1903,8 +1903,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,16 +1931,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1975,10 +1975,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2013,10 +2013,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>